<commit_message>
Update pdf file name
</commit_message>
<xml_diff>
--- a/list/info.xlsx
+++ b/list/info.xlsx
@@ -3,13 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10323"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7364AE5B-86F7-EC40-A394-3157C72640CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BA6BE3-85AF-0B46-914B-3C2B2F0BC308}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="名簿" sheetId="1" r:id="rId1"/>
-    <sheet name="集計" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="114">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1"/>
@@ -112,20 +111,6 @@
       <t>ホゴシャ</t>
     </rPh>
     <rPh sb="3" eb="5">
-      <t>シメイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ID</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>生徒氏名</t>
-    <rPh sb="0" eb="2">
-      <t>セイト</t>
-    </rPh>
-    <rPh sb="2" eb="4">
       <t>シメイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
@@ -1180,12 +1165,13 @@
   <dimension ref="A1:AC14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="P1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="Z11" sqref="Z11"/>
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="8" max="8" width="11.83203125" customWidth="1"/>
     <col min="9" max="9" width="14.1640625" customWidth="1"/>
@@ -1196,7 +1182,7 @@
     <col min="23" max="24" width="13" bestFit="1" customWidth="1"/>
     <col min="25" max="26" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="29" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
@@ -1240,63 +1226,63 @@
         <v>11</v>
       </c>
       <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>20</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>21</v>
       </c>
-      <c r="U1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V1" t="s">
-        <v>23</v>
-      </c>
       <c r="W1" t="s">
+        <v>91</v>
+      </c>
+      <c r="X1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y1" t="s">
         <v>93</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>94</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>95</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>96</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>97</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>98</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:29">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1305,28 +1291,28 @@
         <v>2020</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N2">
         <v>2000</v>
@@ -1338,7 +1324,8 @@
         <v>900</v>
       </c>
       <c r="Q2">
-        <v>100</v>
+        <f>W2*X2</f>
+        <v>150</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -1350,11 +1337,11 @@
         <v>2000</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="V2">
         <f>SUM(N2:U2)</f>
-        <v>6000</v>
+        <v>6950</v>
       </c>
       <c r="W2">
         <v>5</v>
@@ -1363,30 +1350,30 @@
         <v>30</v>
       </c>
       <c r="Y2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="Z2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB2" t="s">
         <v>112</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AC2" t="s">
         <v>113</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:29">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -1395,28 +1382,28 @@
         <v>2021</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N3">
         <v>400</v>
@@ -1428,7 +1415,8 @@
         <v>900</v>
       </c>
       <c r="Q3">
-        <v>300</v>
+        <f t="shared" ref="Q3:Q13" si="0">W3*X3</f>
+        <v>0</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -1443,8 +1431,8 @@
         <v>0</v>
       </c>
       <c r="V3">
-        <f t="shared" ref="V3:V7" si="0">SUM(N3:U3)</f>
-        <v>4600</v>
+        <f t="shared" ref="V3:V7" si="1">SUM(N3:U3)</f>
+        <v>4300</v>
       </c>
       <c r="W3">
         <v>0</v>
@@ -1453,18 +1441,18 @@
         <v>0</v>
       </c>
       <c r="Y3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:29">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D4">
         <v>6</v>
@@ -1473,28 +1461,28 @@
         <v>2020</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N4">
         <v>2390</v>
@@ -1506,7 +1494,8 @@
         <v>900</v>
       </c>
       <c r="Q4">
-        <v>220</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="R4">
         <v>1000</v>
@@ -1521,8 +1510,8 @@
         <v>1000</v>
       </c>
       <c r="V4">
-        <f t="shared" si="0"/>
-        <v>5710</v>
+        <f t="shared" si="1"/>
+        <v>5850</v>
       </c>
       <c r="W4">
         <v>4</v>
@@ -1531,30 +1520,30 @@
         <v>90</v>
       </c>
       <c r="Y4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="Z4" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB4" t="s">
         <v>112</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AC4" t="s">
         <v>113</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>114</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:29">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -1563,28 +1552,28 @@
         <v>2020</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N5">
         <v>3190</v>
@@ -1596,7 +1585,8 @@
         <v>900</v>
       </c>
       <c r="Q5">
-        <v>430</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="R5">
         <v>200</v>
@@ -1611,8 +1601,8 @@
         <v>390</v>
       </c>
       <c r="V5">
-        <f t="shared" si="0"/>
-        <v>6210</v>
+        <f t="shared" si="1"/>
+        <v>5780</v>
       </c>
       <c r="W5">
         <v>0</v>
@@ -1621,21 +1611,21 @@
         <v>0</v>
       </c>
       <c r="Y5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="Z5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:29">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -1644,28 +1634,28 @@
         <v>2021</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="K6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L6" t="s">
         <v>70</v>
       </c>
-      <c r="L6" t="s">
-        <v>72</v>
-      </c>
       <c r="M6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N6">
         <v>5400</v>
@@ -1677,7 +1667,8 @@
         <v>900</v>
       </c>
       <c r="Q6">
-        <v>650</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="R6">
         <v>300</v>
@@ -1689,11 +1680,11 @@
         <v>2000</v>
       </c>
       <c r="U6">
-        <v>450</v>
+        <v>0</v>
       </c>
       <c r="V6">
-        <f t="shared" si="0"/>
-        <v>9900</v>
+        <f t="shared" si="1"/>
+        <v>8800</v>
       </c>
       <c r="W6">
         <v>0</v>
@@ -1702,18 +1693,18 @@
         <v>0</v>
       </c>
       <c r="Y6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:29">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -1722,28 +1713,28 @@
         <v>2021</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L7" t="s">
+        <v>70</v>
+      </c>
+      <c r="M7" t="s">
         <v>71</v>
-      </c>
-      <c r="L7" t="s">
-        <v>72</v>
-      </c>
-      <c r="M7" t="s">
-        <v>73</v>
       </c>
       <c r="N7">
         <v>2230</v>
@@ -1755,7 +1746,8 @@
         <v>1000</v>
       </c>
       <c r="Q7">
-        <v>230</v>
+        <f t="shared" si="0"/>
+        <v>60</v>
       </c>
       <c r="R7">
         <v>0</v>
@@ -1767,11 +1759,11 @@
         <v>1200</v>
       </c>
       <c r="U7">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="V7">
-        <f t="shared" si="0"/>
-        <v>4660</v>
+        <f t="shared" si="1"/>
+        <v>5490</v>
       </c>
       <c r="W7">
         <v>6</v>
@@ -1780,21 +1772,21 @@
         <v>10</v>
       </c>
       <c r="Y7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="Z7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:29">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -1803,28 +1795,28 @@
         <v>2021</v>
       </c>
       <c r="F8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L8" t="s">
+        <v>70</v>
+      </c>
+      <c r="M8" t="s">
         <v>71</v>
-      </c>
-      <c r="L8" t="s">
-        <v>72</v>
-      </c>
-      <c r="M8" t="s">
-        <v>73</v>
       </c>
       <c r="N8">
         <v>2230</v>
@@ -1836,7 +1828,8 @@
         <v>1000</v>
       </c>
       <c r="Q8">
-        <v>230</v>
+        <f t="shared" si="0"/>
+        <v>60</v>
       </c>
       <c r="R8">
         <v>0</v>
@@ -1848,11 +1841,11 @@
         <v>1200</v>
       </c>
       <c r="U8">
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="V8">
-        <f t="shared" ref="V8:V13" si="1">SUM(N8:U8)</f>
-        <v>4660</v>
+        <f t="shared" ref="V8:V13" si="2">SUM(N8:U8)</f>
+        <v>5390</v>
       </c>
       <c r="W8">
         <v>3</v>
@@ -1861,27 +1854,27 @@
         <v>20</v>
       </c>
       <c r="Y8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="Z8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB8" t="s">
         <v>112</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>113</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:29">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D9">
         <v>4</v>
@@ -1890,28 +1883,28 @@
         <v>2020</v>
       </c>
       <c r="F9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L9" t="s">
+        <v>70</v>
+      </c>
+      <c r="M9" t="s">
         <v>71</v>
-      </c>
-      <c r="L9" t="s">
-        <v>72</v>
-      </c>
-      <c r="M9" t="s">
-        <v>73</v>
       </c>
       <c r="N9">
         <v>2230</v>
@@ -1923,7 +1916,8 @@
         <v>1000</v>
       </c>
       <c r="Q9">
-        <v>230</v>
+        <f t="shared" si="0"/>
+        <v>60</v>
       </c>
       <c r="R9">
         <v>0</v>
@@ -1938,8 +1932,8 @@
         <v>0</v>
       </c>
       <c r="V9">
-        <f t="shared" si="1"/>
-        <v>4660</v>
+        <f t="shared" si="2"/>
+        <v>4490</v>
       </c>
       <c r="W9">
         <v>2</v>
@@ -1948,18 +1942,18 @@
         <v>30</v>
       </c>
       <c r="Y9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:29">
       <c r="A10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D10">
         <v>6</v>
@@ -1968,28 +1962,28 @@
         <v>2020</v>
       </c>
       <c r="F10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L10" t="s">
+        <v>70</v>
+      </c>
+      <c r="M10" t="s">
         <v>71</v>
-      </c>
-      <c r="L10" t="s">
-        <v>72</v>
-      </c>
-      <c r="M10" t="s">
-        <v>73</v>
       </c>
       <c r="N10">
         <v>2230</v>
@@ -2001,7 +1995,8 @@
         <v>1000</v>
       </c>
       <c r="Q10">
-        <v>230</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="R10">
         <v>0</v>
@@ -2013,11 +2008,11 @@
         <v>1200</v>
       </c>
       <c r="U10">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="V10">
-        <f t="shared" si="1"/>
-        <v>4660</v>
+        <f t="shared" si="2"/>
+        <v>4730</v>
       </c>
       <c r="W10">
         <v>0</v>
@@ -2026,24 +2021,24 @@
         <v>0</v>
       </c>
       <c r="Y10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="Z10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="AA10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:29">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D11">
         <v>4</v>
@@ -2052,28 +2047,28 @@
         <v>2021</v>
       </c>
       <c r="F11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L11" t="s">
+        <v>70</v>
+      </c>
+      <c r="M11" t="s">
         <v>71</v>
-      </c>
-      <c r="L11" t="s">
-        <v>72</v>
-      </c>
-      <c r="M11" t="s">
-        <v>73</v>
       </c>
       <c r="N11">
         <v>2230</v>
@@ -2085,7 +2080,8 @@
         <v>1000</v>
       </c>
       <c r="Q11">
-        <v>230</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="R11">
         <v>0</v>
@@ -2100,8 +2096,8 @@
         <v>0</v>
       </c>
       <c r="V11">
-        <f t="shared" si="1"/>
-        <v>4660</v>
+        <f t="shared" si="2"/>
+        <v>4430</v>
       </c>
       <c r="W11">
         <v>0</v>
@@ -2110,18 +2106,18 @@
         <v>0</v>
       </c>
       <c r="Y11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:29">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -2130,28 +2126,28 @@
         <v>2019</v>
       </c>
       <c r="F12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L12" t="s">
+        <v>70</v>
+      </c>
+      <c r="M12" t="s">
         <v>71</v>
-      </c>
-      <c r="L12" t="s">
-        <v>72</v>
-      </c>
-      <c r="M12" t="s">
-        <v>73</v>
       </c>
       <c r="N12">
         <v>2230</v>
@@ -2163,7 +2159,8 @@
         <v>1000</v>
       </c>
       <c r="Q12">
-        <v>230</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="R12">
         <v>0</v>
@@ -2178,8 +2175,8 @@
         <v>0</v>
       </c>
       <c r="V12">
-        <f t="shared" si="1"/>
-        <v>4660</v>
+        <f t="shared" si="2"/>
+        <v>4440</v>
       </c>
       <c r="W12">
         <v>1</v>
@@ -2188,18 +2185,18 @@
         <v>10</v>
       </c>
       <c r="Y12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:29">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -2208,28 +2205,28 @@
         <v>2019</v>
       </c>
       <c r="F13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L13" t="s">
+        <v>70</v>
+      </c>
+      <c r="M13" t="s">
         <v>71</v>
-      </c>
-      <c r="L13" t="s">
-        <v>72</v>
-      </c>
-      <c r="M13" t="s">
-        <v>73</v>
       </c>
       <c r="N13">
         <v>2230</v>
@@ -2241,7 +2238,8 @@
         <v>1000</v>
       </c>
       <c r="Q13">
-        <v>230</v>
+        <f t="shared" si="0"/>
+        <v>84</v>
       </c>
       <c r="R13">
         <v>0</v>
@@ -2253,11 +2251,11 @@
         <v>1200</v>
       </c>
       <c r="U13">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="V13">
-        <f t="shared" si="1"/>
-        <v>4660</v>
+        <f t="shared" si="2"/>
+        <v>94514</v>
       </c>
       <c r="W13">
         <v>6</v>
@@ -2266,13 +2264,13 @@
         <v>14</v>
       </c>
       <c r="Y13" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA13" t="s">
         <v>111</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>112</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:29">
@@ -2297,271 +2295,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId13"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K7"/>
-  <sheetViews>
-    <sheetView zoomScale="166" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:K7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
-  <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2">
-        <v>2000</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>900</v>
-      </c>
-      <c r="F2">
-        <v>100</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>1000</v>
-      </c>
-      <c r="I2">
-        <v>2000</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <f>SUM(C2:J2)</f>
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3">
-        <v>400</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>900</v>
-      </c>
-      <c r="F3">
-        <v>300</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>3000</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K7" si="0">SUM(C3:J3)</f>
-        <v>4600</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4">
-        <v>2390</v>
-      </c>
-      <c r="D4">
-        <v>200</v>
-      </c>
-      <c r="E4">
-        <v>900</v>
-      </c>
-      <c r="F4">
-        <v>220</v>
-      </c>
-      <c r="G4">
-        <v>1000</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>1000</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="0"/>
-        <v>5710</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5">
-        <v>3190</v>
-      </c>
-      <c r="D5">
-        <v>100</v>
-      </c>
-      <c r="E5">
-        <v>900</v>
-      </c>
-      <c r="F5">
-        <v>430</v>
-      </c>
-      <c r="G5">
-        <v>200</v>
-      </c>
-      <c r="H5">
-        <v>1000</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>390</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="0"/>
-        <v>6210</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6">
-        <v>5400</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>900</v>
-      </c>
-      <c r="F6">
-        <v>650</v>
-      </c>
-      <c r="G6">
-        <v>300</v>
-      </c>
-      <c r="H6">
-        <v>200</v>
-      </c>
-      <c r="I6">
-        <v>2000</v>
-      </c>
-      <c r="J6">
-        <v>450</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="0"/>
-        <v>9900</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7">
-        <v>2230</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>1000</v>
-      </c>
-      <c r="F7">
-        <v>230</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>1200</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="0"/>
-        <v>4660</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>